<commit_message>
Updates from work during class
</commit_message>
<xml_diff>
--- a/Population by County.xlsx
+++ b/Population by County.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95E5FF4-D28C-41AE-97CE-2F135FE9F56D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7766143-E32D-49B3-A055-107DF3A88A6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="220">
   <si>
     <t>TOTAL POPULATION</t>
   </si>
@@ -778,11 +778,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -1174,7 +1174,7 @@
   </sheetPr>
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A24" sqref="A24:C24"/>
     </sheetView>
   </sheetViews>
@@ -1186,16 +1186,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
@@ -1205,304 +1205,304 @@
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="7"/>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="7"/>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="7"/>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="7"/>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="7"/>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="7"/>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="7"/>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="7"/>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" ht="16.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" ht="56" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="7"/>
     </row>
     <row r="31" spans="1:3" ht="32" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="8"/>
+      <c r="C31" s="7"/>
     </row>
     <row r="32" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="8"/>
+      <c r="C32" s="7"/>
     </row>
     <row r="33" spans="1:3" ht="160.05000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="8"/>
+      <c r="C33" s="7"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
     </row>
     <row r="35" spans="1:3" ht="8" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="8"/>
+      <c r="C35" s="7"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1521,11 +1521,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B265"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1546,1848 +1546,1845 @@
       <c r="A2" s="4" t="s">
         <v>41</v>
       </c>
+      <c r="B2" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>46</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="B8" s="4" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>50</v>
       </c>
+      <c r="B11" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>52</v>
       </c>
+      <c r="B14" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="B17" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>56</v>
       </c>
+      <c r="B20" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>58</v>
       </c>
+      <c r="B23" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>60</v>
       </c>
+      <c r="B26" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>62</v>
       </c>
+      <c r="B29" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="B32" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>66</v>
       </c>
+      <c r="B35" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A38" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="B38" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A39" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A40" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A41" s="4" t="s">
         <v>70</v>
       </c>
+      <c r="B41" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A43" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A44" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="B44" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A45" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A46" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A47" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="B47" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A48" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A49" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A50" s="4" t="s">
         <v>76</v>
       </c>
+      <c r="B50" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A51" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A52" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A53" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="B53" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A54" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A55" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A56" s="4" t="s">
         <v>80</v>
       </c>
+      <c r="B56" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A57" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A58" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A59" s="4" t="s">
         <v>82</v>
       </c>
+      <c r="B59" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A60" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A61" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A62" s="4" t="s">
         <v>84</v>
       </c>
+      <c r="B62" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A63" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A64" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A65" s="4" t="s">
         <v>86</v>
       </c>
+      <c r="B65" s="4" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A66" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A67" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A68" s="4" t="s">
         <v>88</v>
       </c>
+      <c r="B68" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A69" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A70" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A71" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="B71" s="4" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A72" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>91</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A73" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A74" s="4" t="s">
         <v>92</v>
       </c>
+      <c r="B74" s="4" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A75" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A76" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A77" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="B77" s="4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A78" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A79" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A80" s="4" t="s">
         <v>96</v>
       </c>
+      <c r="B80" s="4" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A81" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A82" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A83" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="B83" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A84" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A85" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A86" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="B86" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A87" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A88" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A89" s="4" t="s">
         <v>102</v>
       </c>
+      <c r="B89" s="4" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A90" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>103</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A91" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A92" s="4" t="s">
         <v>104</v>
       </c>
+      <c r="B92" s="4" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A93" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A94" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A95" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="B95" s="4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A96" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A97" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A98" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="B98" s="4" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A99" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>109</v>
+        <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A100" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A101" s="4" t="s">
         <v>110</v>
       </c>
+      <c r="B101" s="4" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A102" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>111</v>
+        <v>45</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A103" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A104" s="4" t="s">
         <v>112</v>
       </c>
+      <c r="B104" s="4" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A105" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>113</v>
+        <v>45</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A106" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A107" s="4" t="s">
         <v>114</v>
       </c>
+      <c r="B107" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A108" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>115</v>
+        <v>45</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A109" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A110" s="4" t="s">
         <v>116</v>
       </c>
+      <c r="B110" s="4" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A111" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>117</v>
+        <v>45</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A112" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" s="4" t="s">
         <v>118</v>
       </c>
+      <c r="B113" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>119</v>
+        <v>45</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B115" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A116" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="B116" s="4" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B118" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" s="4" t="s">
         <v>122</v>
       </c>
+      <c r="B119" s="4" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" s="4" t="s">
         <v>124</v>
       </c>
+      <c r="B122" s="4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="B125" s="4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" s="4" t="s">
         <v>128</v>
       </c>
+      <c r="B128" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>129</v>
+        <v>45</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B130" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" s="4" t="s">
         <v>130</v>
       </c>
+      <c r="B131" s="4" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>131</v>
+        <v>45</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" s="4" t="s">
         <v>132</v>
       </c>
+      <c r="B134" s="4" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B136" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="B137" s="4" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>135</v>
+        <v>45</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B139" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" s="4" t="s">
         <v>136</v>
       </c>
+      <c r="B140" s="4" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>137</v>
+        <v>45</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B142" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" s="4" t="s">
         <v>138</v>
       </c>
+      <c r="B143" s="4" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B145" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A146" s="4" t="s">
         <v>140</v>
       </c>
+      <c r="B146" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>141</v>
+        <v>45</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A148" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B148" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" s="4" t="s">
         <v>142</v>
       </c>
+      <c r="B149" s="4" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A150" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B150" s="4" t="s">
-        <v>143</v>
+        <v>45</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A151" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B151" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A152" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="B152" s="4" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B153" s="4" t="s">
-        <v>145</v>
+        <v>45</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A154" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B154" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A155" s="4" t="s">
         <v>146</v>
       </c>
+      <c r="B155" s="4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A156" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>147</v>
+        <v>45</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A158" s="4" t="s">
         <v>148</v>
       </c>
+      <c r="B158" s="4" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>149</v>
+        <v>45</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A160" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B160" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A161" s="4" t="s">
         <v>150</v>
       </c>
+      <c r="B161" s="4" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A162" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>151</v>
+        <v>45</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A163" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B163" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A164" s="4" t="s">
         <v>152</v>
       </c>
+      <c r="B164" s="4" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A165" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B165" s="4" t="s">
-        <v>153</v>
+        <v>45</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A166" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B166" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A167" s="4" t="s">
         <v>154</v>
       </c>
+      <c r="B167" s="4" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A168" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B168" s="4" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A169" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B169" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A170" s="4" t="s">
         <v>156</v>
       </c>
+      <c r="B170" s="4" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A171" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>157</v>
+        <v>45</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A172" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B172" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A173" s="4" t="s">
         <v>158</v>
       </c>
+      <c r="B173" s="4" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A174" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>159</v>
+        <v>45</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A175" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B175" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A176" s="4" t="s">
         <v>160</v>
       </c>
+      <c r="B176" s="4" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>161</v>
+        <v>45</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A178" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B178" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A179" s="4" t="s">
         <v>162</v>
       </c>
+      <c r="B179" s="4" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A180" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>163</v>
+        <v>45</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A181" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B181" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A182" s="4" t="s">
         <v>164</v>
       </c>
+      <c r="B182" s="4" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A183" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>165</v>
+        <v>45</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A184" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B184" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A185" s="4" t="s">
         <v>166</v>
       </c>
+      <c r="B185" s="4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A186" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>167</v>
+        <v>45</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A187" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B187" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A188" s="4" t="s">
         <v>168</v>
       </c>
+      <c r="B188" s="4" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A189" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A190" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B190" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191" s="4" t="s">
         <v>170</v>
       </c>
+      <c r="B191" s="4" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A192" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>171</v>
+        <v>45</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B193" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A194" s="4" t="s">
         <v>172</v>
       </c>
+      <c r="B194" s="4" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>173</v>
+        <v>45</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A196" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B196" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A197" s="4" t="s">
         <v>174</v>
       </c>
+      <c r="B197" s="4" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A198" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A199" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B199" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A200" s="4" t="s">
         <v>176</v>
       </c>
+      <c r="B200" s="4" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A201" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>177</v>
+        <v>45</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A202" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B202" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A203" s="4" t="s">
         <v>178</v>
       </c>
+      <c r="B203" s="4" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A204" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>179</v>
+        <v>45</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A205" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B205" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A206" s="4" t="s">
         <v>180</v>
       </c>
+      <c r="B206" s="4" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A207" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A208" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B208" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A209" s="4" t="s">
         <v>182</v>
       </c>
+      <c r="B209" s="4" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A210" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B210" s="4" t="s">
-        <v>183</v>
+        <v>45</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A211" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B211" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A212" s="4" t="s">
         <v>184</v>
       </c>
+      <c r="B212" s="4" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A213" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B213" s="4" t="s">
-        <v>185</v>
+        <v>45</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A214" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B214" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A215" s="4" t="s">
         <v>186</v>
       </c>
+      <c r="B215" s="4" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A216" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B216" s="4" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A217" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B217" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A218" s="4" t="s">
         <v>188</v>
       </c>
+      <c r="B218" s="4" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A219" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>189</v>
+        <v>45</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A220" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B220" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A221" s="4" t="s">
         <v>190</v>
       </c>
+      <c r="B221" s="4" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A222" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>191</v>
+        <v>45</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A223" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B223" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A224" s="4" t="s">
         <v>192</v>
       </c>
+      <c r="B224" s="4" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A225" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>193</v>
+        <v>45</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A226" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B226" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A227" s="4" t="s">
         <v>194</v>
       </c>
+      <c r="B227" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A228" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>195</v>
+        <v>45</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A229" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B229" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A230" s="4" t="s">
         <v>196</v>
       </c>
+      <c r="B230" s="4" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A231" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>197</v>
+        <v>45</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A232" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B232" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A233" s="4" t="s">
         <v>198</v>
       </c>
+      <c r="B233" s="4" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A234" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>199</v>
+        <v>45</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A235" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B235" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A236" s="4" t="s">
         <v>200</v>
       </c>
+      <c r="B236" s="4" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A237" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B237" s="4" t="s">
-        <v>201</v>
+        <v>45</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A238" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B238" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A239" s="4" t="s">
         <v>202</v>
       </c>
+      <c r="B239" s="4" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A240" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A241" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B241" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A242" s="4" t="s">
         <v>204</v>
       </c>
+      <c r="B242" s="4" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A243" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B243" s="4" t="s">
-        <v>205</v>
+        <v>45</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A244" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B244" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A245" s="4" t="s">
         <v>206</v>
       </c>
+      <c r="B245" s="4" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A246" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>207</v>
+        <v>45</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A247" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B247" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A248" s="4" t="s">
         <v>208</v>
       </c>
+      <c r="B248" s="4" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A249" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B249" s="4" t="s">
-        <v>209</v>
+        <v>45</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A250" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B250" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A251" s="4" t="s">
         <v>210</v>
       </c>
+      <c r="B251" s="4" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A252" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B252" s="4" t="s">
-        <v>211</v>
+        <v>45</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A253" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B253" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A254" s="4" t="s">
         <v>212</v>
       </c>
+      <c r="B254" s="4" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A255" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B255" s="4" t="s">
-        <v>213</v>
+        <v>45</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A256" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B256" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A257" s="4" t="s">
         <v>214</v>
       </c>
+      <c r="B257" s="4" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A258" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B258" s="4" t="s">
-        <v>215</v>
+        <v>45</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A259" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B259" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A260" s="4" t="s">
         <v>216</v>
       </c>
+      <c r="B260" s="4" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A261" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B261" s="4" t="s">
-        <v>217</v>
+        <v>45</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A262" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B262" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A263" s="4" t="s">
         <v>218</v>
       </c>
+      <c r="B263" s="4" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A264" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B264" s="4" t="s">
-        <v>219</v>
+        <v>45</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A265" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B265" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>